<commit_message>
Made a change to the schema and subsequent changes to the server code
</commit_message>
<xml_diff>
--- a/doc/Design Docs/DB schema.xlsx
+++ b/doc/Design Docs/DB schema.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="9555" windowHeight="6210"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="9552" windowHeight="6216"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Device</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Total Fat</t>
-  </si>
-  <si>
-    <t>Cholsterol</t>
   </si>
   <si>
     <t>Sodium</t>
@@ -72,8 +69,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +146,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -227,6 +229,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -261,6 +264,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -436,42 +440,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:N4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14">
-      <c r="B4" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1</v>
@@ -505,9 +508,6 @@
       </c>
       <c r="M4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -517,24 +517,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>